<commit_message>
Fixed Untagged getting marked as matchrow
Applies update() to untagged pivot to change PIVOT_MARK to PIVOT
</commit_message>
<xml_diff>
--- a/monitoring_sample.xlsx
+++ b/monitoring_sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="file_monitoring" sheetId="1" r:id="rId1"/>
@@ -728,7 +728,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -739,8 +739,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,7 +973,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AQ1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>